<commit_message>
View Contamination Hits not highlighting features with cfu #45
</commit_message>
<xml_diff>
--- a/other_resources/doc/TOTS_schemas.xlsx
+++ b/other_resources/doc/TOTS_schemas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PDziemiela\Documents\GitHub\EPA-HSRP-TOTS\other_resources\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B802BE1E-8246-4EFE-81A9-24457E5C6CB7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5AE1B9-5627-4D63-9A99-46571BF9DF5D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-300" windowWidth="16440" windowHeight="28440" activeTab="3" xr2:uid="{3B4DA81F-2C02-47FA-BEC8-B0DA6FF9909F}"/>
+    <workbookView xWindow="-16320" yWindow="-300" windowWidth="16440" windowHeight="28440" xr2:uid="{3B4DA81F-2C02-47FA-BEC8-B0DA6FF9909F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sampling Event" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="112">
   <si>
     <t>Sampling Event</t>
   </si>
@@ -740,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF39B3FB-52A5-4B1E-A480-5EB23EB5EB87}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="A1:F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,37 +972,37 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
-      </c>
-      <c r="D16" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
         <v>14</v>
+      </c>
+      <c r="D17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
@@ -1010,111 +1010,102 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20">
-        <v>2000</v>
-      </c>
-      <c r="D20" t="s">
-        <v>77</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="C21">
+        <v>2000</v>
       </c>
       <c r="D21" t="s">
-        <v>78</v>
-      </c>
-      <c r="E21" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>30</v>
       </c>
-      <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" t="s">
         <v>79</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E23" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>12</v>
       </c>
-      <c r="C23">
+      <c r="C24">
         <v>255</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>80</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E24" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" t="s">
-        <v>81</v>
-      </c>
-      <c r="E24" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
         <v>32</v>
       </c>
       <c r="D25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>60</v>
-      </c>
-      <c r="B26" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26">
-        <v>255</v>
-      </c>
-      <c r="D26" t="s">
-        <v>35</v>
-      </c>
-      <c r="E26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="B27" t="s">
         <v>12</v>
@@ -1123,43 +1114,60 @@
         <v>255</v>
       </c>
       <c r="D27" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E27" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>62</v>
+      <c r="A28" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="B28" t="s">
         <v>12</v>
       </c>
       <c r="C28">
-        <v>16</v>
+        <v>255</v>
       </c>
       <c r="D28" t="s">
-        <v>83</v>
+        <v>37</v>
       </c>
       <c r="E28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B29" t="s">
         <v>12</v>
       </c>
       <c r="C29">
+        <v>16</v>
+      </c>
+      <c r="D29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30">
         <v>255</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>84</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E30" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1393,7 +1401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05F98EAB-C6C6-422C-929B-6A73BD5F5BF8}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -1598,21 +1606,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BC45D02C15A2B94E9866BE6472EB2DCD" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e3915ffdcdffce6c03d48ff5f59cfc3a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="918453a5-0c81-4647-9315-d1d1382281b3" xmlns:ns3="c9f57a8e-870f-49f8-9eae-a12f43fb5efa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b474895ef806082062b167af6bdb1cc7" ns2:_="" ns3:_="">
     <xsd:import namespace="918453a5-0c81-4647-9315-d1d1382281b3"/>
@@ -1817,24 +1810,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BD68529-960B-4507-AB86-A5506EBDE60B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC247834-2741-4F68-88FC-BBB05EEBC3F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{401CA379-A056-4AE1-B22C-A7E65207052B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1851,4 +1842,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC247834-2741-4F68-88FC-BBB05EEBC3F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BD68529-960B-4507-AB86-A5506EBDE60B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
changes to record layout
</commit_message>
<xml_diff>
--- a/other_resources/doc/TOTS_schemas.xlsx
+++ b/other_resources/doc/TOTS_schemas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PDziemiela\Documents\GitHub\EPA-HSRP-TOTS\other_resources\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16ED4F0F-7CF3-4195-A0AB-178C277A824F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE9FCD8-4660-4B4C-A46D-B183CBA83552}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3B4DA81F-2C02-47FA-BEC8-B0DA6FF9909F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="142">
   <si>
     <t>Sampling Event</t>
   </si>
@@ -126,9 +126,6 @@
     <t>AMC</t>
   </si>
   <si>
-    <t>Sample this Main script provides this value as a header to the CSV report</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -288,9 +285,6 @@
     <t>Elevation Series</t>
   </si>
   <si>
-    <t>CFU</t>
-  </si>
-  <si>
     <t>Contamination Map</t>
   </si>
   <si>
@@ -385,6 +379,87 @@
   </si>
   <si>
     <t>40-byte global unique identifier for the area of interest object.</t>
+  </si>
+  <si>
+    <t>Assigned at creation</t>
+  </si>
+  <si>
+    <t>Esri Managed</t>
+  </si>
+  <si>
+    <t>But in future should be Esri managed</t>
+  </si>
+  <si>
+    <t>Are there scenarios where TYPE can change?</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Calculated</t>
+  </si>
+  <si>
+    <t>What is ITER???</t>
+  </si>
+  <si>
+    <t>Optional Scenario Name</t>
+  </si>
+  <si>
+    <t>Bump when record is changed</t>
+  </si>
+  <si>
+    <t>CONTAM_UNIT</t>
+  </si>
+  <si>
+    <t>Contamination Unit</t>
+  </si>
+  <si>
+    <t>CONTAM_TYPE</t>
+  </si>
+  <si>
+    <t>Contamination Type</t>
+  </si>
+  <si>
+    <t>Keyword describing the type of contamination in the map</t>
+  </si>
+  <si>
+    <t>Description useful for organizing contamination maps</t>
+  </si>
+  <si>
+    <t>Notes on the given record</t>
+  </si>
+  <si>
+    <t>Unit used in describing the contamination measurement</t>
+  </si>
+  <si>
+    <t>Value of the contamination located in the polygon</t>
+  </si>
+  <si>
+    <t>Do we have domain of possible values?</t>
+  </si>
+  <si>
+    <t>Contamination Map Type</t>
+  </si>
+  <si>
+    <t>Assigned by GP tool</t>
+  </si>
+  <si>
+    <t>Contamination Map Value</t>
+  </si>
+  <si>
+    <t>Contamination Map Unit</t>
+  </si>
+  <si>
+    <t>I feel we cannot ever mix units for a given map</t>
+  </si>
+  <si>
+    <t>Description useful for organizing areas of interest</t>
+  </si>
+  <si>
+    <t>CONTAM_VALUE</t>
+  </si>
+  <si>
+    <t>Contamination Value</t>
   </si>
 </sst>
 </file>
@@ -755,11 +830,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF39B3FB-52A5-4B1E-A480-5EB23EB5EB87}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -768,19 +841,20 @@
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="28.28515625" customWidth="1"/>
     <col min="5" max="5" width="70.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="31.42578125" customWidth="1"/>
+    <col min="7" max="7" width="38.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="str">
-        <f>"March 6, 2020"</f>
-        <v>March 6, 2020</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <f>"March 17, 2020"</f>
+        <v>March 17, 2020</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -791,18 +865,21 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -811,12 +888,15 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="F3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -825,24 +905,33 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="F4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -853,13 +942,19 @@
         <v>255</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="F6" t="s">
+        <v>115</v>
+      </c>
+      <c r="G6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -867,13 +962,16 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -881,13 +979,16 @@
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -895,13 +996,16 @@
         <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="F9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -909,13 +1013,16 @@
         <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="F10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -923,13 +1030,13 @@
         <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -937,13 +1044,13 @@
         <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -951,13 +1058,16 @@
         <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="F13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -965,13 +1075,16 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="F14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -979,13 +1092,13 @@
         <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -993,75 +1106,90 @@
         <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
         <v>13</v>
       </c>
-      <c r="D18" t="s">
-        <v>75</v>
-      </c>
-      <c r="E18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C21">
+        <v>2000</v>
+      </c>
+      <c r="D21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22">
-        <v>2000</v>
+        <v>13</v>
       </c>
       <c r="D22" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
         <v>13</v>
@@ -1070,122 +1198,156 @@
         <v>77</v>
       </c>
       <c r="E23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="3">
+        <v>64</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F24" t="s">
+        <v>119</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D24" t="s">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F25" t="s">
+        <v>119</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="3">
+        <v>64</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F26" t="s">
+        <v>119</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27">
+        <v>255</v>
+      </c>
+      <c r="D27" t="s">
         <v>78</v>
       </c>
-      <c r="E24" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="E27" t="s">
+        <v>122</v>
+      </c>
+      <c r="F27" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>56</v>
       </c>
-      <c r="B25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25">
-        <v>255</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" t="s">
         <v>79</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F28" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="D29" t="s">
         <v>80</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E29" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="F29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>58</v>
-      </c>
-      <c r="B27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D27" t="s">
-        <v>81</v>
-      </c>
-      <c r="E27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28">
-        <v>255</v>
-      </c>
-      <c r="D28" t="s">
-        <v>34</v>
-      </c>
-      <c r="E28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29">
-        <v>255</v>
-      </c>
-      <c r="D29" t="s">
-        <v>36</v>
-      </c>
-      <c r="E29" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>61</v>
       </c>
       <c r="B30" t="s">
         <v>11</v>
       </c>
       <c r="C30">
-        <v>16</v>
+        <v>255</v>
       </c>
       <c r="D30" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E30" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>62</v>
+        <v>34</v>
+      </c>
+      <c r="F30" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="B31" t="s">
         <v>11</v>
@@ -1194,10 +1356,53 @@
         <v>255</v>
       </c>
       <c r="D31" t="s">
-        <v>83</v>
+        <v>35</v>
       </c>
       <c r="E31" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="F31" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32">
+        <v>16</v>
+      </c>
+      <c r="D32" t="s">
+        <v>81</v>
+      </c>
+      <c r="E32" t="s">
+        <v>37</v>
+      </c>
+      <c r="F32" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33">
+        <v>255</v>
+      </c>
+      <c r="D33" t="s">
+        <v>82</v>
+      </c>
+      <c r="E33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F33" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1208,31 +1413,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D5FB865-8BEA-4E52-93D1-84C264A59DBB}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E4"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="29.28515625" customWidth="1"/>
     <col min="5" max="5" width="55.140625" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" customWidth="1"/>
+    <col min="7" max="7" width="40.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F1" t="str">
-        <f>"March 6, 2020"</f>
-        <v>March 6, 2020</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <f>'Sampling Event'!F1</f>
+        <v>March 17, 2020</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1243,18 +1450,21 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -1263,12 +1473,15 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="F3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -1277,57 +1490,133 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="F4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>56</v>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>126</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6">
-        <v>255</v>
+        <v>64</v>
       </c>
       <c r="D6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="E6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F6" t="s">
+        <v>115</v>
+      </c>
+      <c r="G6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>84</v>
+        <v>140</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>27</v>
+      <c r="D7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E7" t="s">
+        <v>132</v>
+      </c>
+      <c r="F7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8">
+        <v>64</v>
+      </c>
+      <c r="D8" t="s">
+        <v>125</v>
+      </c>
+      <c r="E8" t="s">
+        <v>131</v>
+      </c>
+      <c r="F8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
         <v>255</v>
       </c>
-      <c r="D8" t="s">
-        <v>76</v>
+      <c r="D9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" t="s">
+        <v>130</v>
+      </c>
+      <c r="F9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>255</v>
+      </c>
+      <c r="D10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" t="s">
+        <v>129</v>
+      </c>
+      <c r="F10" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1337,10 +1626,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A2189D3-90CD-43CC-9932-8D77872EECB4}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,19 +1638,21 @@
     <col min="2" max="2" width="9.7109375" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="29.28515625" customWidth="1"/>
-    <col min="5" max="5" width="51.7109375" customWidth="1"/>
+    <col min="5" max="5" width="57.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" customWidth="1"/>
+    <col min="7" max="7" width="35.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F1" t="str">
-        <f>"March 6, 2020"</f>
-        <v>March 6, 2020</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <f>'Sampling Event'!F1</f>
+        <v>March 17, 2020</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1372,18 +1663,21 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -1392,12 +1686,15 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="F3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -1406,26 +1703,35 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="F4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>56</v>
+        <v>114</v>
+      </c>
+      <c r="F5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -1434,12 +1740,18 @@
         <v>255</v>
       </c>
       <c r="D6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>27</v>
+        <v>75</v>
+      </c>
+      <c r="E6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -1448,7 +1760,13 @@
         <v>255</v>
       </c>
       <c r="D7" t="s">
-        <v>76</v>
+        <v>78</v>
+      </c>
+      <c r="E7" t="s">
+        <v>139</v>
+      </c>
+      <c r="F7" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1461,7 +1779,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1476,11 +1794,11 @@
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F1" t="str">
-        <f>"March 6, 2020"</f>
-        <v>March 6, 2020</v>
+        <f>'Sampling Event'!F1</f>
+        <v>March 17, 2020</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1494,18 +1812,18 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -1514,12 +1832,12 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -1527,18 +1845,18 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
@@ -1546,7 +1864,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
@@ -1554,7 +1872,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -1562,7 +1880,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -1570,7 +1888,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
@@ -1578,7 +1896,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -1587,56 +1905,56 @@
         <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" t="s">
         <v>99</v>
       </c>
-      <c r="D13" t="s">
-        <v>101</v>
-      </c>
       <c r="E13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
@@ -1645,18 +1963,18 @@
         <v>40</v>
       </c>
       <c r="D16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1665,21 +1983,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BC45D02C15A2B94E9866BE6472EB2DCD" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e3915ffdcdffce6c03d48ff5f59cfc3a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="918453a5-0c81-4647-9315-d1d1382281b3" xmlns:ns3="c9f57a8e-870f-49f8-9eae-a12f43fb5efa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b474895ef806082062b167af6bdb1cc7" ns2:_="" ns3:_="">
     <xsd:import namespace="918453a5-0c81-4647-9315-d1d1382281b3"/>
@@ -1884,24 +2187,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BD68529-960B-4507-AB86-A5506EBDE60B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC247834-2741-4F68-88FC-BBB05EEBC3F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{401CA379-A056-4AE1-B22C-A7E65207052B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1918,4 +2219,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC247834-2741-4F68-88FC-BBB05EEBC3F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BD68529-960B-4507-AB86-A5506EBDE60B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added sampling metthods from spreadsheet, add AA and AC descriptions
</commit_message>
<xml_diff>
--- a/other_resources/doc/TOTS_schemas.xlsx
+++ b/other_resources/doc/TOTS_schemas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PDziemiela\Documents\GitHub\EPA-HSRP-TOTS\other_resources\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\EPA-HSRP-TOTS\other_resources\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE9FCD8-4660-4B4C-A46D-B183CBA83552}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E6CA7F-40D4-4337-A28F-C267B5BC9D6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3B4DA81F-2C02-47FA-BEC8-B0DA6FF9909F}"/>
+    <workbookView xWindow="-28920" yWindow="-2460" windowWidth="29040" windowHeight="15840" xr2:uid="{3B4DA81F-2C02-47FA-BEC8-B0DA6FF9909F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sampling Event" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Area of Interest" sheetId="3" r:id="rId3"/>
     <sheet name="Old VSP" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="154">
   <si>
     <t>Sampling Event</t>
   </si>
@@ -177,9 +179,6 @@
     <t>Waste Weight per Sample (lbs)</t>
   </si>
   <si>
-    <t>Sampling Method: Swab, Sponge, MicroVac,</t>
-  </si>
-  <si>
     <t>Analysis Material Cost (US dollars)</t>
   </si>
   <si>
@@ -258,9 +257,6 @@
     <t>Waste Weight per Sample</t>
   </si>
   <si>
-    <t>Sampling Surface Area</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -460,13 +456,55 @@
   </si>
   <si>
     <t>Contamination Value</t>
+  </si>
+  <si>
+    <t>Caleb's Comments</t>
+  </si>
+  <si>
+    <t>Not currently</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I believe this was just a loop counter in the original code and it was used to execute some code on the 1st iteration only. I'm not using this at all and it can be removed. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I think this one is should be considered a variable. It is a hardcoded value per sample. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I think this one is should be considered a variable. It is a hardcoded value per sample. This isn't being used for anything other than just being displayed in the popup. Can this be removed? </t>
+  </si>
+  <si>
+    <t>I don't think there is any reason for this attribute to exist. Now that the calculations are on the client side, this is not being saved to the graphic's attributes.</t>
+  </si>
+  <si>
+    <t>This variable isn't being used for anything other than just being displayed in the popup.</t>
+  </si>
+  <si>
+    <t>This variable isn't being used for anything other than just being displayed in the popup and on the calculate results panel.</t>
+  </si>
+  <si>
+    <t>Sampling Method: Swab, Sponge, Wipe, Micro-Vacuum, Sponge-Wipe  Composite, Micro-Vacuum Composite, Robotic Floor Cleaner, Grab/Bulk, Water sample, Wet Vacuum)</t>
+  </si>
+  <si>
+    <t>Area (sq inch)</t>
+  </si>
+  <si>
+    <t>Sampling Surface Area (sq inch)</t>
+  </si>
+  <si>
+    <t>Area (sq inches) / Surface Area (sq inch); if Area &lt; Surface Area, then AC = 1</t>
+  </si>
+  <si>
+    <t>Area (sq inches) / Surface Area (sq inch)</t>
+  </si>
+  <si>
+    <t>iteration, always =1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -486,6 +524,13 @@
     <font>
       <sz val="20"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -511,11 +556,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -830,9 +876,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF39B3FB-52A5-4B1E-A480-5EB23EB5EB87}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -840,12 +888,13 @@
     <col min="2" max="2" width="9.7109375" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="28.28515625" customWidth="1"/>
-    <col min="5" max="5" width="70.140625" customWidth="1"/>
-    <col min="6" max="6" width="31.42578125" customWidth="1"/>
-    <col min="7" max="7" width="38.140625" customWidth="1"/>
+    <col min="5" max="5" width="57.5703125" customWidth="1"/>
+    <col min="6" max="6" width="29" customWidth="1"/>
+    <col min="7" max="7" width="41" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="171.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -854,7 +903,7 @@
         <v>March 17, 2020</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -865,21 +914,24 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -888,15 +940,15 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -905,33 +957,33 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G4" t="s">
         <v>115</v>
       </c>
-      <c r="G4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -942,19 +994,22 @@
         <v>255</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>148</v>
       </c>
       <c r="F6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="H6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -962,16 +1017,16 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E7" t="s">
         <v>39</v>
       </c>
       <c r="F7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -979,16 +1034,16 @@
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E8" t="s">
         <v>40</v>
       </c>
       <c r="F8" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -996,16 +1051,16 @@
         <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E9" t="s">
         <v>41</v>
       </c>
       <c r="F9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1013,16 +1068,16 @@
         <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E10" t="s">
         <v>42</v>
       </c>
       <c r="F10" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1030,13 +1085,16 @@
         <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="H11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1044,13 +1102,16 @@
         <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="H12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1064,10 +1125,10 @@
         <v>43</v>
       </c>
       <c r="F13" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1075,16 +1136,19 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E14" t="s">
         <v>44</v>
       </c>
       <c r="F14" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="H14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1092,13 +1156,16 @@
         <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E15" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1106,13 +1173,16 @@
         <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E16" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1120,43 +1190,67 @@
         <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>74</v>
+        <v>150</v>
       </c>
       <c r="E17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F17" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="H17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
       <c r="B18" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D18" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H18" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D19" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E19" t="s">
+        <v>151</v>
+      </c>
+      <c r="H19" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
       </c>
+      <c r="E20" t="s">
+        <v>153</v>
+      </c>
       <c r="F20" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="H20" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1167,10 +1261,10 @@
         <v>2000</v>
       </c>
       <c r="D21" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1178,16 +1272,19 @@
         <v>13</v>
       </c>
       <c r="D22" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F22" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="H22" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1195,18 +1292,21 @@
         <v>13</v>
       </c>
       <c r="D23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F23" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="H23" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>11</v>
@@ -1215,42 +1315,42 @@
         <v>64</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F24" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F25" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>11</v>
@@ -1259,21 +1359,21 @@
         <v>64</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F26" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
         <v>11</v>
@@ -1282,52 +1382,52 @@
         <v>255</v>
       </c>
       <c r="D27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F27" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
         <v>30</v>
       </c>
       <c r="D28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E28" t="s">
         <v>31</v>
       </c>
       <c r="F28" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B29" t="s">
         <v>30</v>
       </c>
       <c r="D29" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E29" t="s">
         <v>32</v>
       </c>
       <c r="F29" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B30" t="s">
         <v>11</v>
@@ -1342,12 +1442,12 @@
         <v>34</v>
       </c>
       <c r="F30" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B31" t="s">
         <v>11</v>
@@ -1362,12 +1462,12 @@
         <v>36</v>
       </c>
       <c r="F31" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B32" t="s">
         <v>11</v>
@@ -1376,18 +1476,18 @@
         <v>16</v>
       </c>
       <c r="D32" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E32" t="s">
         <v>37</v>
       </c>
       <c r="F32" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B33" t="s">
         <v>11</v>
@@ -1396,13 +1496,13 @@
         <v>255</v>
       </c>
       <c r="D33" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E33" t="s">
         <v>38</v>
       </c>
       <c r="F33" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1432,7 +1532,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F1" t="str">
         <f>'Sampling Event'!F1</f>
@@ -1450,21 +1550,21 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -1473,15 +1573,15 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -1490,35 +1590,35 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G4" t="s">
         <v>115</v>
-      </c>
-      <c r="G4" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F5" t="s">
         <v>113</v>
-      </c>
-      <c r="F5" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -1527,38 +1627,38 @@
         <v>64</v>
       </c>
       <c r="D6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -1567,16 +1667,16 @@
         <v>64</v>
       </c>
       <c r="D8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1590,18 +1690,18 @@
         <v>255</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -1610,13 +1710,13 @@
         <v>255</v>
       </c>
       <c r="D10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1645,7 +1745,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F1" t="str">
         <f>'Sampling Event'!F1</f>
@@ -1663,21 +1763,21 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -1686,15 +1786,15 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -1703,30 +1803,30 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G4" t="s">
         <v>115</v>
-      </c>
-      <c r="G4" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1740,18 +1840,18 @@
         <v>255</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -1760,13 +1860,13 @@
         <v>255</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1794,7 +1894,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F1" t="str">
         <f>'Sampling Event'!F1</f>
@@ -1812,18 +1912,18 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -1832,12 +1932,12 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -1845,18 +1945,18 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
@@ -1864,7 +1964,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
@@ -1872,7 +1972,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -1880,7 +1980,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -1888,7 +1988,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
@@ -1896,7 +1996,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -1905,56 +2005,56 @@
         <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" t="s">
         <v>97</v>
       </c>
-      <c r="D13" t="s">
-        <v>99</v>
-      </c>
       <c r="E13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
@@ -1963,18 +2063,18 @@
         <v>40</v>
       </c>
       <c r="D16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1983,6 +2083,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BC45D02C15A2B94E9866BE6472EB2DCD" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e3915ffdcdffce6c03d48ff5f59cfc3a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="918453a5-0c81-4647-9315-d1d1382281b3" xmlns:ns3="c9f57a8e-870f-49f8-9eae-a12f43fb5efa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b474895ef806082062b167af6bdb1cc7" ns2:_="" ns3:_="">
     <xsd:import namespace="918453a5-0c81-4647-9315-d1d1382281b3"/>
@@ -2187,22 +2302,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC247834-2741-4F68-88FC-BBB05EEBC3F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BD68529-960B-4507-AB86-A5506EBDE60B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="918453a5-0c81-4647-9315-d1d1382281b3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c9f57a8e-870f-49f8-9eae-a12f43fb5efa"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{401CA379-A056-4AE1-B22C-A7E65207052B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2219,21 +2344,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC247834-2741-4F68-88FC-BBB05EEBC3F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BD68529-960B-4507-AB86-A5506EBDE60B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
changes to contamination layer attrb
</commit_message>
<xml_diff>
--- a/other_resources/doc/TOTS_schemas.xlsx
+++ b/other_resources/doc/TOTS_schemas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\EPA-HSRP-TOTS\other_resources\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E6CA7F-40D4-4337-A28F-C267B5BC9D6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542AC824-8275-4B70-B588-40D4368A0528}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2460" windowWidth="29040" windowHeight="15840" xr2:uid="{3B4DA81F-2C02-47FA-BEC8-B0DA6FF9909F}"/>
+    <workbookView xWindow="-28920" yWindow="-2460" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3B4DA81F-2C02-47FA-BEC8-B0DA6FF9909F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sampling Event" sheetId="1" r:id="rId1"/>
@@ -431,9 +431,6 @@
     <t>Value of the contamination located in the polygon</t>
   </si>
   <si>
-    <t>Do we have domain of possible values?</t>
-  </si>
-  <si>
     <t>Contamination Map Type</t>
   </si>
   <si>
@@ -446,9 +443,6 @@
     <t>Contamination Map Unit</t>
   </si>
   <si>
-    <t>I feel we cannot ever mix units for a given map</t>
-  </si>
-  <si>
     <t>Description useful for organizing areas of interest</t>
   </si>
   <si>
@@ -498,6 +492,13 @@
   </si>
   <si>
     <t>iteration, always =1</t>
+  </si>
+  <si>
+    <t>chemical, radiological, biological</t>
+  </si>
+  <si>
+    <t>ALR - We should use domain values 
+PTD - I feel we cannot ever mix units for a given map</t>
   </si>
 </sst>
 </file>
@@ -556,12 +557,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -878,7 +882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF39B3FB-52A5-4B1E-A480-5EB23EB5EB87}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -926,7 +930,7 @@
         <v>73</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -997,7 +1001,7 @@
         <v>61</v>
       </c>
       <c r="E6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F6" t="s">
         <v>113</v>
@@ -1006,7 +1010,7 @@
         <v>116</v>
       </c>
       <c r="H6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1091,7 +1095,7 @@
         <v>68</v>
       </c>
       <c r="H11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1108,7 +1112,7 @@
         <v>67</v>
       </c>
       <c r="H12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1145,7 +1149,7 @@
         <v>118</v>
       </c>
       <c r="H14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1162,7 +1166,7 @@
         <v>45</v>
       </c>
       <c r="H15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1179,7 +1183,7 @@
         <v>46</v>
       </c>
       <c r="H16" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1190,7 +1194,7 @@
         <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E17" t="s">
         <v>50</v>
@@ -1199,7 +1203,7 @@
         <v>118</v>
       </c>
       <c r="H17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1210,10 +1214,10 @@
         <v>13</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1224,13 +1228,13 @@
         <v>6</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E19" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1241,13 +1245,13 @@
         <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F20" t="s">
         <v>119</v>
       </c>
       <c r="H20" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1281,7 +1285,7 @@
         <v>118</v>
       </c>
       <c r="H22" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1301,7 +1305,7 @@
         <v>118</v>
       </c>
       <c r="H23" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1318,34 +1322,34 @@
         <v>125</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F24" t="s">
         <v>117</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F25" t="s">
         <v>117</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1362,13 +1366,13 @@
         <v>123</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F26" t="s">
         <v>117</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1515,8 +1519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D5FB865-8BEA-4E52-93D1-84C264A59DBB}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G10:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1636,18 +1640,18 @@
         <v>113</v>
       </c>
       <c r="G6" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E7" t="s">
         <v>130</v>
@@ -1656,7 +1660,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>122</v>
       </c>
@@ -1675,8 +1679,8 @@
       <c r="F8" t="s">
         <v>113</v>
       </c>
-      <c r="G8" t="s">
-        <v>136</v>
+      <c r="G8" s="5" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1863,7 +1867,7 @@
         <v>76</v>
       </c>
       <c r="E7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F7" t="s">
         <v>113</v>
@@ -2083,18 +2087,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2303,14 +2307,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC247834-2741-4F68-88FC-BBB05EEBC3F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BD68529-960B-4507-AB86-A5506EBDE60B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -2323,6 +2319,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="c9f57a8e-870f-49f8-9eae-a12f43fb5efa"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC247834-2741-4F68-88FC-BBB05EEBC3F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updated the descriptions for SA and AA in the TOTS_schemas spreadsheet.
</commit_message>
<xml_diff>
--- a/other_resources/doc/TOTS_schemas.xlsx
+++ b/other_resources/doc/TOTS_schemas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\EPA-HSRP-TOTS\other_resources\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TOTS\EPA-HSRP-TOTS-commit-test\other_resources\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542AC824-8275-4B70-B588-40D4368A0528}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A8D578-85F3-47BD-8A19-7A60A0AC44BE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2460" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3B4DA81F-2C02-47FA-BEC8-B0DA6FF9909F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3B4DA81F-2C02-47FA-BEC8-B0DA6FF9909F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sampling Event" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="155">
   <si>
     <t>Sampling Event</t>
   </si>
@@ -186,9 +184,6 @@
   </si>
   <si>
     <t>Source</t>
-  </si>
-  <si>
-    <t>Sampling Surface Area (sq inches)</t>
   </si>
   <si>
     <t>Alias</t>
@@ -499,6 +494,12 @@
   <si>
     <t>ALR - We should use domain values 
 PTD - I feel we cannot ever mix units for a given map</t>
+  </si>
+  <si>
+    <t>Sampling Surface Area (sq inches) required for the sample type</t>
+  </si>
+  <si>
+    <t>Actual area of user specified sample</t>
   </si>
 </sst>
 </file>
@@ -882,8 +883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF39B3FB-52A5-4B1E-A480-5EB23EB5EB87}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,7 +919,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
@@ -927,15 +928,15 @@
         <v>49</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -944,15 +945,15 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -961,30 +962,30 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -998,19 +999,19 @@
         <v>255</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1021,13 +1022,13 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E7" t="s">
         <v>39</v>
       </c>
       <c r="F7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1038,13 +1039,13 @@
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
         <v>40</v>
       </c>
       <c r="F8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1055,13 +1056,13 @@
         <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E9" t="s">
         <v>41</v>
       </c>
       <c r="F9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1072,13 +1073,13 @@
         <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E10" t="s">
         <v>42</v>
       </c>
       <c r="F10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1089,13 +1090,13 @@
         <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1106,13 +1107,13 @@
         <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1129,7 +1130,7 @@
         <v>43</v>
       </c>
       <c r="F13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1140,16 +1141,16 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E14" t="s">
         <v>44</v>
       </c>
       <c r="F14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1160,13 +1161,13 @@
         <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E15" t="s">
         <v>45</v>
       </c>
       <c r="H15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1177,13 +1178,13 @@
         <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E16" t="s">
         <v>46</v>
       </c>
       <c r="H16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1194,16 +1195,16 @@
         <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E17" t="s">
-        <v>50</v>
+        <v>153</v>
       </c>
       <c r="F17" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1214,10 +1215,16 @@
         <v>13</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
+      </c>
+      <c r="E18" t="s">
+        <v>154</v>
+      </c>
+      <c r="F18" t="s">
+        <v>117</v>
       </c>
       <c r="H18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1228,13 +1235,13 @@
         <v>6</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1245,13 +1252,13 @@
         <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1265,7 +1272,7 @@
         <v>2000</v>
       </c>
       <c r="D21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1276,16 +1283,16 @@
         <v>13</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E22" t="s">
         <v>48</v>
       </c>
       <c r="F22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1296,21 +1303,21 @@
         <v>13</v>
       </c>
       <c r="D23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E23" t="s">
         <v>47</v>
       </c>
       <c r="F23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>11</v>
@@ -1319,42 +1326,42 @@
         <v>64</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E24" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F24" t="s">
+        <v>116</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="F24" t="s">
-        <v>117</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>11</v>
@@ -1363,21 +1370,21 @@
         <v>64</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B27" t="s">
         <v>11</v>
@@ -1386,52 +1393,52 @@
         <v>255</v>
       </c>
       <c r="D27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
         <v>30</v>
       </c>
       <c r="D28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E28" t="s">
         <v>31</v>
       </c>
       <c r="F28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B29" t="s">
         <v>30</v>
       </c>
       <c r="D29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E29" t="s">
         <v>32</v>
       </c>
       <c r="F29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B30" t="s">
         <v>11</v>
@@ -1446,12 +1453,12 @@
         <v>34</v>
       </c>
       <c r="F30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B31" t="s">
         <v>11</v>
@@ -1466,12 +1473,12 @@
         <v>36</v>
       </c>
       <c r="F31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B32" t="s">
         <v>11</v>
@@ -1480,18 +1487,18 @@
         <v>16</v>
       </c>
       <c r="D32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E32" t="s">
         <v>37</v>
       </c>
       <c r="F32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B33" t="s">
         <v>11</v>
@@ -1500,13 +1507,13 @@
         <v>255</v>
       </c>
       <c r="D33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E33" t="s">
         <v>38</v>
       </c>
       <c r="F33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1519,8 +1526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D5FB865-8BEA-4E52-93D1-84C264A59DBB}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G10:G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1536,7 +1543,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F1" t="str">
         <f>'Sampling Event'!F1</f>
@@ -1554,7 +1561,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
@@ -1563,12 +1570,12 @@
         <v>49</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -1577,15 +1584,15 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -1594,35 +1601,35 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -1631,38 +1638,38 @@
         <v>64</v>
       </c>
       <c r="D6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E6" t="s">
         <v>125</v>
       </c>
-      <c r="E6" t="s">
-        <v>126</v>
-      </c>
       <c r="F6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -1671,16 +1678,16 @@
         <v>64</v>
       </c>
       <c r="D8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1694,18 +1701,18 @@
         <v>255</v>
       </c>
       <c r="D9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -1714,13 +1721,13 @@
         <v>255</v>
       </c>
       <c r="D10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1749,7 +1756,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F1" t="str">
         <f>'Sampling Event'!F1</f>
@@ -1767,7 +1774,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
@@ -1776,12 +1783,12 @@
         <v>49</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -1790,15 +1797,15 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -1807,30 +1814,30 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F5" t="s">
         <v>112</v>
-      </c>
-      <c r="F5" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1844,18 +1851,18 @@
         <v>255</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -1864,13 +1871,13 @@
         <v>255</v>
       </c>
       <c r="D7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1898,7 +1905,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F1" t="str">
         <f>'Sampling Event'!F1</f>
@@ -1916,7 +1923,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
@@ -1927,7 +1934,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -1936,12 +1943,12 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -1949,18 +1956,18 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
@@ -1968,7 +1975,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
@@ -1976,7 +1983,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -1984,7 +1991,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -1992,7 +1999,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
@@ -2000,7 +2007,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -2009,56 +2016,56 @@
         <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" t="s">
         <v>94</v>
-      </c>
-      <c r="B12" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" t="s">
         <v>96</v>
       </c>
-      <c r="B13" t="s">
-        <v>95</v>
-      </c>
-      <c r="D13" t="s">
-        <v>97</v>
-      </c>
       <c r="E13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" t="s">
         <v>98</v>
-      </c>
-      <c r="B14" t="s">
-        <v>95</v>
-      </c>
-      <c r="D14" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" t="s">
         <v>100</v>
-      </c>
-      <c r="B15" t="s">
-        <v>95</v>
-      </c>
-      <c r="D15" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
@@ -2067,18 +2074,18 @@
         <v>40</v>
       </c>
       <c r="D16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2087,21 +2094,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BC45D02C15A2B94E9866BE6472EB2DCD" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e3915ffdcdffce6c03d48ff5f59cfc3a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="918453a5-0c81-4647-9315-d1d1382281b3" xmlns:ns3="c9f57a8e-870f-49f8-9eae-a12f43fb5efa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b474895ef806082062b167af6bdb1cc7" ns2:_="" ns3:_="">
     <xsd:import namespace="918453a5-0c81-4647-9315-d1d1382281b3"/>
@@ -2306,32 +2298,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BD68529-960B-4507-AB86-A5506EBDE60B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="918453a5-0c81-4647-9315-d1d1382281b3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c9f57a8e-870f-49f8-9eae-a12f43fb5efa"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC247834-2741-4F68-88FC-BBB05EEBC3F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{401CA379-A056-4AE1-B22C-A7E65207052B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2348,4 +2330,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC247834-2741-4F68-88FC-BBB05EEBC3F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BD68529-960B-4507-AB86-A5506EBDE60B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="918453a5-0c81-4647-9315-d1d1382281b3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c9f57a8e-870f-49f8-9eae-a12f43fb5efa"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Made some changes to required fields (for upload) in red for Sample layer
</commit_message>
<xml_diff>
--- a/other_resources/doc/TOTS_schemas.xlsx
+++ b/other_resources/doc/TOTS_schemas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TOTS\EPA-HSRP-TOTS-commit-test\other_resources\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\EPA-HSRP-TOTS\other_resources\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A8D578-85F3-47BD-8A19-7A60A0AC44BE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F044633-BD29-4385-8249-635D4430E741}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3B4DA81F-2C02-47FA-BEC8-B0DA6FF9909F}"/>
+    <workbookView xWindow="20370" yWindow="-3255" windowWidth="29040" windowHeight="15840" xr2:uid="{3B4DA81F-2C02-47FA-BEC8-B0DA6FF9909F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sampling Event" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="155">
   <si>
     <t>Sampling Event</t>
   </si>
@@ -506,7 +508,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -531,6 +533,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -558,15 +583,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -884,7 +912,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="A6" activeCellId="1" sqref="A21:A23 A6:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,22 +1017,22 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="5">
         <v>255</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="5" t="s">
         <v>112</v>
       </c>
       <c r="G6" t="s">
@@ -1015,192 +1043,211 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="5" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D8" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="5" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D9" t="s">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="5" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D10" t="s">
+      <c r="C10" s="5"/>
+      <c r="D10" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="5" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D11" t="s">
+      <c r="C11" s="5"/>
+      <c r="D11" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="5" t="s">
         <v>67</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>116</v>
       </c>
       <c r="H11" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D12" t="s">
+      <c r="C12" s="5"/>
+      <c r="D12" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="5" t="s">
         <v>66</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>116</v>
       </c>
       <c r="H12" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D13" t="s">
+      <c r="C13" s="5"/>
+      <c r="D13" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="5" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D14" t="s">
+      <c r="C14" s="5"/>
+      <c r="D14" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F14" t="s">
-        <v>117</v>
+      <c r="F14" s="5" t="s">
+        <v>116</v>
       </c>
       <c r="H14" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D15" t="s">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="5" t="s">
         <v>45</v>
       </c>
+      <c r="F15" s="5"/>
       <c r="H15" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D16" t="s">
+      <c r="C16" s="5"/>
+      <c r="D16" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="5" t="s">
         <v>46</v>
       </c>
+      <c r="F16" s="5"/>
       <c r="H16" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D17" t="s">
+      <c r="C17" s="6"/>
+      <c r="D17" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="6" t="s">
         <v>116</v>
       </c>
       <c r="H17" t="s">
@@ -1208,19 +1255,20 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="C18" s="6"/>
+      <c r="D18" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="6" t="s">
         <v>117</v>
       </c>
       <c r="H18" t="s">
@@ -1228,88 +1276,94 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="C19" s="6"/>
+      <c r="D19" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="6" t="s">
         <v>148</v>
       </c>
+      <c r="F19" s="6"/>
       <c r="H19" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="6" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="5">
         <v>2000</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="5" t="s">
         <v>72</v>
       </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D22" t="s">
+      <c r="C22" s="5"/>
+      <c r="D22" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F22" t="s">
-        <v>117</v>
+      <c r="F22" s="5" t="s">
+        <v>116</v>
       </c>
       <c r="H22" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D23" t="s">
+      <c r="C23" s="5"/>
+      <c r="D23" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F23" t="s">
-        <v>117</v>
+      <c r="F23" s="5" t="s">
+        <v>116</v>
       </c>
       <c r="H23" t="s">
         <v>140</v>
@@ -1383,22 +1437,22 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="6">
         <v>255</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="6" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1686,7 +1740,7 @@
       <c r="F8" t="s">
         <v>112</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2299,18 +2353,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2333,14 +2387,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC247834-2741-4F68-88FC-BBB05EEBC3F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BD68529-960B-4507-AB86-A5506EBDE60B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -2355,4 +2401,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC247834-2741-4F68-88FC-BBB05EEBC3F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
#85 Updated the spreadsheet to reflect that SA is a required field.
</commit_message>
<xml_diff>
--- a/other_resources/doc/TOTS_schemas.xlsx
+++ b/other_resources/doc/TOTS_schemas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\EPA-HSRP-TOTS\other_resources\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TOTS\EPA-HSRP-TOTS\other_resources\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F044633-BD29-4385-8249-635D4430E741}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C25977-7CE4-4F70-8573-DEBE28C010E2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-3255" windowWidth="29040" windowHeight="15840" xr2:uid="{3B4DA81F-2C02-47FA-BEC8-B0DA6FF9909F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3B4DA81F-2C02-47FA-BEC8-B0DA6FF9909F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sampling Event" sheetId="1" r:id="rId1"/>
@@ -912,7 +912,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" activeCellId="1" sqref="A21:A23 A6:A16"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1234,20 +1234,20 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6" t="s">
+      <c r="C17" s="5"/>
+      <c r="D17" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="5" t="s">
         <v>116</v>
       </c>
       <c r="H17" t="s">
@@ -1271,7 +1271,7 @@
       <c r="F18" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="6" t="s">
         <v>142</v>
       </c>
     </row>
@@ -1290,7 +1290,7 @@
         <v>148</v>
       </c>
       <c r="F19" s="6"/>
-      <c r="H19" t="s">
+      <c r="H19" s="6" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2148,6 +2148,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BC45D02C15A2B94E9866BE6472EB2DCD" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e3915ffdcdffce6c03d48ff5f59cfc3a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="918453a5-0c81-4647-9315-d1d1382281b3" xmlns:ns3="c9f57a8e-870f-49f8-9eae-a12f43fb5efa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b474895ef806082062b167af6bdb1cc7" ns2:_="" ns3:_="">
     <xsd:import namespace="918453a5-0c81-4647-9315-d1d1382281b3"/>
@@ -2352,36 +2367,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{401CA379-A056-4AE1-B22C-A7E65207052B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC247834-2741-4F68-88FC-BBB05EEBC3F7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="918453a5-0c81-4647-9315-d1d1382281b3"/>
-    <ds:schemaRef ds:uri="c9f57a8e-870f-49f8-9eae-a12f43fb5efa"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2404,9 +2393,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC247834-2741-4F68-88FC-BBB05EEBC3F7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{401CA379-A056-4AE1-B22C-A7E65207052B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="918453a5-0c81-4647-9315-d1d1382281b3"/>
+    <ds:schemaRef ds:uri="c9f57a8e-870f-49f8-9eae-a12f43fb5efa"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Changed field names for CONTAM as shapefiles only support 10 char fieldnames
</commit_message>
<xml_diff>
--- a/other_resources/doc/TOTS_schemas.xlsx
+++ b/other_resources/doc/TOTS_schemas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TOTS\EPA-HSRP-TOTS\other_resources\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\EPA-HSRP-TOTS\other_resources\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C25977-7CE4-4F70-8573-DEBE28C010E2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC316FBC-514C-40DA-B592-F497D2EC76DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3B4DA81F-2C02-47FA-BEC8-B0DA6FF9909F}"/>
+    <workbookView xWindow="20370" yWindow="-3255" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3B4DA81F-2C02-47FA-BEC8-B0DA6FF9909F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sampling Event" sheetId="1" r:id="rId1"/>
@@ -401,15 +401,9 @@
     <t>Bump when record is changed</t>
   </si>
   <si>
-    <t>CONTAM_UNIT</t>
-  </si>
-  <si>
     <t>Contamination Unit</t>
   </si>
   <si>
-    <t>CONTAM_TYPE</t>
-  </si>
-  <si>
     <t>Contamination Type</t>
   </si>
   <si>
@@ -443,9 +437,6 @@
     <t>Description useful for organizing areas of interest</t>
   </si>
   <si>
-    <t>CONTAM_VALUE</t>
-  </si>
-  <si>
     <t>Contamination Value</t>
   </si>
   <si>
@@ -494,14 +485,23 @@
     <t>chemical, radiological, biological</t>
   </si>
   <si>
-    <t>ALR - We should use domain values 
+    <t>Sampling Surface Area (sq inches) required for the sample type</t>
+  </si>
+  <si>
+    <t>Actual area of user specified sample</t>
+  </si>
+  <si>
+    <t>CONTAMTYPE</t>
+  </si>
+  <si>
+    <t>CONTAMVAL</t>
+  </si>
+  <si>
+    <t>CONTAMUNIT</t>
+  </si>
+  <si>
+    <t>ALR - We should use domain values. Only acceptable value is CFU
 PTD - I feel we cannot ever mix units for a given map</t>
-  </si>
-  <si>
-    <t>Sampling Surface Area (sq inches) required for the sample type</t>
-  </si>
-  <si>
-    <t>Actual area of user specified sample</t>
   </si>
 </sst>
 </file>
@@ -911,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF39B3FB-52A5-4B1E-A480-5EB23EB5EB87}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,7 +959,7 @@
         <v>72</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1030,7 +1030,7 @@
         <v>60</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>112</v>
@@ -1039,7 +1039,7 @@
         <v>115</v>
       </c>
       <c r="H6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1132,7 +1132,7 @@
         <v>116</v>
       </c>
       <c r="H11" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1153,7 +1153,7 @@
         <v>116</v>
       </c>
       <c r="H12" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1192,7 +1192,7 @@
         <v>116</v>
       </c>
       <c r="H14" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1211,7 +1211,7 @@
       </c>
       <c r="F15" s="5"/>
       <c r="H15" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1230,7 +1230,7 @@
       </c>
       <c r="F16" s="5"/>
       <c r="H16" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1242,16 +1242,16 @@
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>116</v>
       </c>
       <c r="H17" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1263,16 +1263,16 @@
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>117</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1284,14 +1284,14 @@
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F19" s="6"/>
       <c r="H19" s="6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1302,13 +1302,13 @@
         <v>6</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>118</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1345,7 +1345,7 @@
         <v>116</v>
       </c>
       <c r="H22" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1366,74 +1366,74 @@
         <v>116</v>
       </c>
       <c r="H23" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="3">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F24" t="s">
         <v>116</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F25" t="s">
         <v>116</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>121</v>
+        <v>153</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="3">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F26" t="s">
         <v>116</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1580,8 +1580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D5FB865-8BEA-4E52-93D1-84C264A59DBB}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G13:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1683,65 +1683,65 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F6" t="s">
         <v>112</v>
       </c>
       <c r="G6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>121</v>
+        <v>153</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F8" t="s">
         <v>112</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1758,7 +1758,7 @@
         <v>72</v>
       </c>
       <c r="E9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F9" t="s">
         <v>112</v>
@@ -1778,7 +1778,7 @@
         <v>75</v>
       </c>
       <c r="E10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F10" t="s">
         <v>112</v>
@@ -1908,7 +1908,7 @@
         <v>72</v>
       </c>
       <c r="E6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F6" t="s">
         <v>112</v>
@@ -1928,7 +1928,7 @@
         <v>75</v>
       </c>
       <c r="E7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F7" t="s">
         <v>112</v>
@@ -2148,18 +2148,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2368,14 +2368,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC247834-2741-4F68-88FC-BBB05EEBC3F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BD68529-960B-4507-AB86-A5506EBDE60B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -2388,6 +2380,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="c9f57a8e-870f-49f8-9eae-a12f43fb5efa"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC247834-2741-4F68-88FC-BBB05EEBC3F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
add sample type record layout
</commit_message>
<xml_diff>
--- a/other_resources/doc/TOTS_schemas.xlsx
+++ b/other_resources/doc/TOTS_schemas.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\EPA-HSRP-TOTS\other_resources\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PDziemiela\Documents\GitHub\EPA-HSRP-TOTS\other_resources\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC316FBC-514C-40DA-B592-F497D2EC76DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5048E8F2-9DFC-4214-AA68-95414A1C7028}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-3255" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3B4DA81F-2C02-47FA-BEC8-B0DA6FF9909F}"/>
+    <workbookView xWindow="20625" yWindow="90" windowWidth="24495" windowHeight="15270" activeTab="4" xr2:uid="{3B4DA81F-2C02-47FA-BEC8-B0DA6FF9909F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sampling Event" sheetId="1" r:id="rId1"/>
     <sheet name="Contamination Map" sheetId="2" r:id="rId2"/>
     <sheet name="Area of Interest" sheetId="3" r:id="rId3"/>
     <sheet name="Old VSP" sheetId="4" r:id="rId4"/>
+    <sheet name="Sample Type" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="152">
   <si>
     <t>Sampling Event</t>
   </si>
@@ -110,15 +111,6 @@
     <t>SA</t>
   </si>
   <si>
-    <t>AA</t>
-  </si>
-  <si>
-    <t>AC</t>
-  </si>
-  <si>
-    <t>ITER</t>
-  </si>
-  <si>
     <t>NOTES</t>
   </si>
   <si>
@@ -389,15 +381,6 @@
     <t>Variable</t>
   </si>
   <si>
-    <t>Calculated</t>
-  </si>
-  <si>
-    <t>What is ITER???</t>
-  </si>
-  <si>
-    <t>Optional Scenario Name</t>
-  </si>
-  <si>
     <t>Bump when record is changed</t>
   </si>
   <si>
@@ -446,9 +429,6 @@
     <t>Not currently</t>
   </si>
   <si>
-    <t xml:space="preserve">I believe this was just a loop counter in the original code and it was used to execute some code on the 1st iteration only. I'm not using this at all and it can be removed. </t>
-  </si>
-  <si>
     <t xml:space="preserve">I think this one is should be considered a variable. It is a hardcoded value per sample. </t>
   </si>
   <si>
@@ -467,28 +447,13 @@
     <t>Sampling Method: Swab, Sponge, Wipe, Micro-Vacuum, Sponge-Wipe  Composite, Micro-Vacuum Composite, Robotic Floor Cleaner, Grab/Bulk, Water sample, Wet Vacuum)</t>
   </si>
   <si>
-    <t>Area (sq inch)</t>
-  </si>
-  <si>
     <t>Sampling Surface Area (sq inch)</t>
   </si>
   <si>
-    <t>Area (sq inches) / Surface Area (sq inch); if Area &lt; Surface Area, then AC = 1</t>
-  </si>
-  <si>
-    <t>Area (sq inches) / Surface Area (sq inch)</t>
-  </si>
-  <si>
-    <t>iteration, always =1</t>
-  </si>
-  <si>
     <t>chemical, radiological, biological</t>
   </si>
   <si>
     <t>Sampling Surface Area (sq inches) required for the sample type</t>
-  </si>
-  <si>
-    <t>Actual area of user specified sample</t>
   </si>
   <si>
     <t>CONTAMTYPE</t>
@@ -502,13 +467,40 @@
   <si>
     <t>ALR - We should use domain values. Only acceptable value is CFU
 PTD - I feel we cannot ever mix units for a given map</t>
+  </si>
+  <si>
+    <t>Sample Type</t>
+  </si>
+  <si>
+    <t>40-byte global unique identifier for the sampling type</t>
+  </si>
+  <si>
+    <t>Sampling Type Name</t>
+  </si>
+  <si>
+    <t>AUTHORITY</t>
+  </si>
+  <si>
+    <t>Authority</t>
+  </si>
+  <si>
+    <t>Free text establishing authority or ownership of sample type parameters</t>
+  </si>
+  <si>
+    <t>Human-friendly Sample Type Name</t>
+  </si>
+  <si>
+    <t>Assigned at creation, change if record is altered by user</t>
+  </si>
+  <si>
+    <t>Assigned at creation, blank/alter if changed by user</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -539,29 +531,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -583,7 +552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -592,9 +561,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -909,10 +875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF39B3FB-52A5-4B1E-A480-5EB23EB5EB87}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,24 +913,24 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -973,15 +939,15 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -990,30 +956,30 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1027,19 +993,19 @@
         <v>255</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="F6" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G6" t="s">
         <v>112</v>
       </c>
-      <c r="G6" t="s">
-        <v>115</v>
-      </c>
       <c r="H6" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1051,13 +1017,13 @@
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1069,13 +1035,13 @@
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1087,13 +1053,13 @@
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1105,13 +1071,13 @@
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1123,16 +1089,16 @@
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H11" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1144,16 +1110,16 @@
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H12" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1165,13 +1131,13 @@
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1183,16 +1149,16 @@
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H14" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1204,14 +1170,14 @@
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F15" s="5"/>
       <c r="H15" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1223,14 +1189,14 @@
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F16" s="5"/>
       <c r="H16" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1242,332 +1208,255 @@
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="F17" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="H17" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="H19" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="H20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="3">
+        <v>20</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="H17" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="F19" s="6"/>
-      <c r="H19" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="E21" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F21" t="s">
+        <v>113</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F22" t="s">
+        <v>113</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="3">
+        <v>10</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F23" t="s">
+        <v>113</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="D24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="H22" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="H23" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="C26">
+        <v>255</v>
+      </c>
+      <c r="D26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="3">
-        <v>20</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="F24" t="s">
-        <v>116</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="F25" t="s">
-        <v>116</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="3">
-        <v>10</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F26" t="s">
-        <v>116</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="6">
+      <c r="C27">
         <v>255</v>
       </c>
-      <c r="D27" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>112</v>
+      <c r="D27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>11</v>
+      </c>
+      <c r="C28">
+        <v>16</v>
       </c>
       <c r="D28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E28" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F28" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>11</v>
+      </c>
+      <c r="C29">
+        <v>255</v>
       </c>
       <c r="D29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E29" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F29" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30">
-        <v>255</v>
-      </c>
-      <c r="D30" t="s">
-        <v>33</v>
-      </c>
-      <c r="E30" t="s">
-        <v>34</v>
-      </c>
-      <c r="F30" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31">
-        <v>255</v>
-      </c>
-      <c r="D31" t="s">
-        <v>35</v>
-      </c>
-      <c r="E31" t="s">
-        <v>36</v>
-      </c>
-      <c r="F31" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>58</v>
-      </c>
-      <c r="B32" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32">
-        <v>16</v>
-      </c>
-      <c r="D32" t="s">
-        <v>78</v>
-      </c>
-      <c r="E32" t="s">
-        <v>37</v>
-      </c>
-      <c r="F32" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>59</v>
-      </c>
-      <c r="B33" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33">
-        <v>255</v>
-      </c>
-      <c r="D33" t="s">
-        <v>79</v>
-      </c>
-      <c r="E33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F33" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1580,8 +1469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D5FB865-8BEA-4E52-93D1-84C264A59DBB}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G13:G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1597,7 +1486,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F1" t="str">
         <f>'Sampling Event'!F1</f>
@@ -1615,21 +1504,21 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -1638,15 +1527,15 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -1655,35 +1544,35 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" t="s">
         <v>107</v>
       </c>
-      <c r="E5" t="s">
-        <v>110</v>
-      </c>
       <c r="F5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -1692,38 +1581,38 @@
         <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E6" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G6" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E7" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -1732,21 +1621,21 @@
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="E8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -1755,18 +1644,18 @@
         <v>255</v>
       </c>
       <c r="D9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -1775,13 +1664,13 @@
         <v>255</v>
       </c>
       <c r="D10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E10" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F10" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1810,7 +1699,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F1" t="str">
         <f>'Sampling Event'!F1</f>
@@ -1828,21 +1717,21 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -1851,15 +1740,15 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -1868,35 +1757,35 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -1905,18 +1794,18 @@
         <v>255</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E6" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -1925,13 +1814,13 @@
         <v>255</v>
       </c>
       <c r="D7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E7" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="F7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1944,7 +1833,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G1" sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1959,7 +1848,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F1" t="str">
         <f>'Sampling Event'!F1</f>
@@ -1977,18 +1866,18 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -1997,12 +1886,12 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -2010,18 +1899,18 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
@@ -2029,7 +1918,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
@@ -2037,7 +1926,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -2045,7 +1934,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -2053,7 +1942,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
@@ -2061,7 +1950,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -2070,56 +1959,56 @@
         <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D13" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E13" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B14" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D14" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
@@ -2128,18 +2017,429 @@
         <v>40</v>
       </c>
       <c r="D16" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
       <c r="D17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B663E0B-3E91-411C-9E0C-70B9C75DEEF4}">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" customWidth="1"/>
+    <col min="5" max="5" width="70.140625" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" t="str">
+        <f>"August 27, 2020"</f>
+        <v>August 27, 2020</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
         <v>104</v>
+      </c>
+      <c r="E5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>255</v>
+      </c>
+      <c r="D6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>136</v>
+      </c>
+      <c r="E15" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22">
+        <v>255</v>
+      </c>
+      <c r="D22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>146</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23">
+        <v>255</v>
+      </c>
+      <c r="D23" t="s">
+        <v>147</v>
+      </c>
+      <c r="E23" t="s">
+        <v>148</v>
+      </c>
+      <c r="F23" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24">
+        <v>255</v>
+      </c>
+      <c r="D24" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" t="s">
+        <v>119</v>
+      </c>
+      <c r="F24" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the TOTS_schemas doc.
</commit_message>
<xml_diff>
--- a/other_resources/doc/TOTS_schemas.xlsx
+++ b/other_resources/doc/TOTS_schemas.xlsx
@@ -5,19 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PDziemiela\Documents\GitHub\EPA-HSRP-TOTS\other_resources\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TOTS\EPA-HSRP-TOTS\other_resources\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5048E8F2-9DFC-4214-AA68-95414A1C7028}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55789CE-1B7F-4C6F-AB99-E323BF7B9610}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20625" yWindow="90" windowWidth="24495" windowHeight="15270" activeTab="4" xr2:uid="{3B4DA81F-2C02-47FA-BEC8-B0DA6FF9909F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3B4DA81F-2C02-47FA-BEC8-B0DA6FF9909F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sampling Event" sheetId="1" r:id="rId1"/>
     <sheet name="Contamination Map" sheetId="2" r:id="rId2"/>
     <sheet name="Area of Interest" sheetId="3" r:id="rId3"/>
     <sheet name="Old VSP" sheetId="4" r:id="rId4"/>
-    <sheet name="Sample Type" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="147">
   <si>
     <t>Sampling Event</t>
   </si>
@@ -144,9 +143,6 @@
     <t>Reiterate the units used for measuring (ft2)</t>
   </si>
   <si>
-    <t>Grouping key indicative of height or elevation or building floor</t>
-  </si>
-  <si>
     <t>Time to Prepare Kits (person hours per sample)</t>
   </si>
   <si>
@@ -207,9 +203,6 @@
     <t>SURFACEAREAUNIT</t>
   </si>
   <si>
-    <t>ELEVATIONSERIES</t>
-  </si>
-  <si>
     <t>Sampling Method Type</t>
   </si>
   <si>
@@ -267,9 +260,6 @@
     <t>Surface Area Unit</t>
   </si>
   <si>
-    <t>Elevation Series</t>
-  </si>
-  <si>
     <t>Contamination Map</t>
   </si>
   <si>
@@ -375,9 +365,6 @@
     <t>But in future should be Esri managed</t>
   </si>
   <si>
-    <t>Are there scenarios where TYPE can change?</t>
-  </si>
-  <si>
     <t>Variable</t>
   </si>
   <si>
@@ -421,27 +408,6 @@
   </si>
   <si>
     <t>Contamination Value</t>
-  </si>
-  <si>
-    <t>Caleb's Comments</t>
-  </si>
-  <si>
-    <t>Not currently</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I think this one is should be considered a variable. It is a hardcoded value per sample. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">I think this one is should be considered a variable. It is a hardcoded value per sample. This isn't being used for anything other than just being displayed in the popup. Can this be removed? </t>
-  </si>
-  <si>
-    <t>I don't think there is any reason for this attribute to exist. Now that the calculations are on the client side, this is not being saved to the graphic's attributes.</t>
-  </si>
-  <si>
-    <t>This variable isn't being used for anything other than just being displayed in the popup.</t>
-  </si>
-  <si>
-    <t>This variable isn't being used for anything other than just being displayed in the popup and on the calculate results panel.</t>
   </si>
   <si>
     <t>Sampling Method: Swab, Sponge, Wipe, Micro-Vacuum, Sponge-Wipe  Composite, Micro-Vacuum Composite, Robotic Floor Cleaner, Grab/Bulk, Water sample, Wet Vacuum)</t>
@@ -469,31 +435,49 @@
 PTD - I feel we cannot ever mix units for a given map</t>
   </si>
   <si>
-    <t>Sample Type</t>
-  </si>
-  <si>
-    <t>40-byte global unique identifier for the sampling type</t>
-  </si>
-  <si>
-    <t>Sampling Type Name</t>
-  </si>
-  <si>
-    <t>AUTHORITY</t>
-  </si>
-  <si>
-    <t>Authority</t>
-  </si>
-  <si>
-    <t>Free text establishing authority or ownership of sample type parameters</t>
-  </si>
-  <si>
-    <t>Human-friendly Sample Type Name</t>
-  </si>
-  <si>
-    <t>Assigned at creation, change if record is altered by user</t>
-  </si>
-  <si>
-    <t>Assigned at creation, blank/alter if changed by user</t>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>Actual Area (sq inch)</t>
+  </si>
+  <si>
+    <t>Surface Area (sq inches) that was measured by TOTS</t>
+  </si>
+  <si>
+    <t>Assigned by TOTS and published to AGO</t>
+  </si>
+  <si>
+    <t>DECISIONUNITUUID</t>
+  </si>
+  <si>
+    <t>Decision Unit UUID</t>
+  </si>
+  <si>
+    <t>40-byte global unique identifier for the sampling layer.</t>
+  </si>
+  <si>
+    <t>DECISIONUNIT</t>
+  </si>
+  <si>
+    <t>Decision Unit</t>
+  </si>
+  <si>
+    <t>Grouping key indicative of sample layer. This could be elevation, building floor, location, etc.</t>
+  </si>
+  <si>
+    <t>DECISIONUNITSORT</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Decision Unit Sort</t>
+  </si>
+  <si>
+    <t>Controls how decision units (layers) are ordered in TOTS.</t>
+  </si>
+  <si>
+    <t>Currently not used. But will be in a future release of TOTS.</t>
   </si>
 </sst>
 </file>
@@ -875,10 +859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF39B3FB-52A5-4B1E-A480-5EB23EB5EB87}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,14 +870,13 @@
     <col min="1" max="1" width="23.42578125" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="57.5703125" customWidth="1"/>
     <col min="6" max="6" width="29" customWidth="1"/>
-    <col min="7" max="7" width="41" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="171.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -902,7 +885,7 @@
         <v>March 17, 2020</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -913,24 +896,21 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -939,15 +919,15 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -956,33 +936,33 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -993,22 +973,16 @@
         <v>255</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="G6" t="s">
-        <v>112</v>
-      </c>
-      <c r="H6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -1017,16 +991,16 @@
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1035,16 +1009,16 @@
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
@@ -1053,16 +1027,16 @@
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
@@ -1071,16 +1045,16 @@
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>17</v>
       </c>
@@ -1089,19 +1063,16 @@
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="F11" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="H11" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>18</v>
       </c>
@@ -1110,19 +1081,16 @@
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="H12" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>19</v>
       </c>
@@ -1131,16 +1099,16 @@
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>20</v>
       </c>
@@ -1149,19 +1117,16 @@
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="H14" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>21</v>
       </c>
@@ -1170,17 +1135,16 @@
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="5"/>
-      <c r="H15" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>22</v>
       </c>
@@ -1189,17 +1153,16 @@
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F16" s="5"/>
-      <c r="H16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>23</v>
       </c>
@@ -1208,200 +1171,192 @@
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="H17" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="B18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B19" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C19" s="5">
         <v>2000</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="D19" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="H19" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>44</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="H20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="3">
+        <v>20</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F22" t="s">
+        <v>109</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F23" t="s">
+        <v>109</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B21" s="3" t="s">
+      <c r="B24" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="3">
-        <v>20</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="F21" t="s">
-        <v>113</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="F22" t="s">
-        <v>113</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="3">
+      <c r="C24" s="3">
         <v>10</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="F23" t="s">
-        <v>113</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" t="s">
-        <v>73</v>
-      </c>
-      <c r="E24" t="s">
-        <v>28</v>
+      <c r="D24" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="F24" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G24" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s">
         <v>27</v>
       </c>
       <c r="D25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E26" t="s">
         <v>29</v>
       </c>
-      <c r="F25" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26">
-        <v>255</v>
-      </c>
-      <c r="D26" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26" t="s">
-        <v>31</v>
-      </c>
       <c r="F26" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>54</v>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>52</v>
       </c>
       <c r="B27" t="s">
         <v>11</v>
@@ -1410,53 +1365,110 @@
         <v>255</v>
       </c>
       <c r="D27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E27" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F27" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>55</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="B28" t="s">
         <v>11</v>
       </c>
       <c r="C28">
-        <v>16</v>
+        <v>255</v>
       </c>
       <c r="D28" t="s">
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="E28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F28" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B29" t="s">
         <v>11</v>
       </c>
       <c r="C29">
+        <v>16</v>
+      </c>
+      <c r="D29" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29" t="s">
+        <v>34</v>
+      </c>
+      <c r="F29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>137</v>
+      </c>
+      <c r="E30" t="s">
+        <v>138</v>
+      </c>
+      <c r="F30" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>139</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31">
         <v>255</v>
       </c>
-      <c r="D29" t="s">
-        <v>76</v>
-      </c>
-      <c r="E29" t="s">
-        <v>35</v>
-      </c>
-      <c r="F29" t="s">
-        <v>113</v>
+      <c r="D31" t="s">
+        <v>140</v>
+      </c>
+      <c r="E31" t="s">
+        <v>141</v>
+      </c>
+      <c r="F31" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>142</v>
+      </c>
+      <c r="B32" t="s">
+        <v>143</v>
+      </c>
+      <c r="D32" t="s">
+        <v>144</v>
+      </c>
+      <c r="E32" t="s">
+        <v>145</v>
+      </c>
+      <c r="F32" t="s">
+        <v>109</v>
+      </c>
+      <c r="G32" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1486,7 +1498,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F1" t="str">
         <f>'Sampling Event'!F1</f>
@@ -1504,21 +1516,21 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -1527,15 +1539,15 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -1544,35 +1556,35 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" t="s">
         <v>104</v>
       </c>
-      <c r="E5" t="s">
-        <v>107</v>
-      </c>
       <c r="F5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -1581,38 +1593,38 @@
         <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E6" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G6" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E7" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -1621,16 +1633,16 @@
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E8" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1644,18 +1656,18 @@
         <v>255</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E9" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -1664,13 +1676,13 @@
         <v>255</v>
       </c>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E10" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F10" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1699,7 +1711,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F1" t="str">
         <f>'Sampling Event'!F1</f>
@@ -1717,21 +1729,21 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -1740,15 +1752,15 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -1757,30 +1769,30 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1794,18 +1806,18 @@
         <v>255</v>
       </c>
       <c r="D6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -1814,13 +1826,13 @@
         <v>255</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1848,7 +1860,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F1" t="str">
         <f>'Sampling Event'!F1</f>
@@ -1866,18 +1878,18 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -1886,12 +1898,12 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -1899,18 +1911,18 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
@@ -1918,7 +1930,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
@@ -1926,7 +1938,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -1934,7 +1946,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -1942,7 +1954,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
@@ -1950,7 +1962,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -1959,56 +1971,56 @@
         <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B14" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D14" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D15" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
@@ -2017,429 +2029,18 @@
         <v>40</v>
       </c>
       <c r="D16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>101</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B663E0B-3E91-411C-9E0C-70B9C75DEEF4}">
-  <dimension ref="A1:G24"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" customWidth="1"/>
-    <col min="5" max="5" width="70.140625" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F1" t="str">
-        <f>"August 27, 2020"</f>
-        <v>August 27, 2020</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>105</v>
-      </c>
-      <c r="F4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>104</v>
-      </c>
-      <c r="E5" t="s">
-        <v>144</v>
-      </c>
-      <c r="F5" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6">
-        <v>255</v>
-      </c>
-      <c r="D6" t="s">
-        <v>145</v>
-      </c>
-      <c r="E6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" t="s">
-        <v>136</v>
-      </c>
-      <c r="E15" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" t="s">
-        <v>70</v>
-      </c>
-      <c r="E16" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" t="s">
-        <v>71</v>
-      </c>
-      <c r="E17" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18" t="s">
-        <v>64</v>
-      </c>
-      <c r="F18" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" t="s">
-        <v>65</v>
-      </c>
-      <c r="E19" t="s">
-        <v>63</v>
-      </c>
-      <c r="F19" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" t="s">
-        <v>73</v>
-      </c>
-      <c r="E20" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" t="s">
-        <v>74</v>
-      </c>
-      <c r="E21" t="s">
-        <v>29</v>
-      </c>
-      <c r="F21" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22">
-        <v>255</v>
-      </c>
-      <c r="D22" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22" t="s">
-        <v>31</v>
-      </c>
-      <c r="F22" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>146</v>
-      </c>
-      <c r="B23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23">
-        <v>255</v>
-      </c>
-      <c r="D23" t="s">
-        <v>147</v>
-      </c>
-      <c r="E23" t="s">
-        <v>148</v>
-      </c>
-      <c r="F23" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24">
-        <v>255</v>
-      </c>
-      <c r="D24" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" t="s">
-        <v>119</v>
-      </c>
-      <c r="F24" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2448,18 +2049,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2668,6 +2269,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC247834-2741-4F68-88FC-BBB05EEBC3F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BD68529-960B-4507-AB86-A5506EBDE60B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -2680,14 +2289,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="c9f57a8e-870f-49f8-9eae-a12f43fb5efa"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC247834-2741-4F68-88FC-BBB05EEBC3F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>